<commit_message>
Updated to include fractional beta power
</commit_message>
<xml_diff>
--- a/fig2/data/Figure_2_boxplot_data.xlsx
+++ b/fig2/data/Figure_2_boxplot_data.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25915"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21126"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gittis\Documents\GitHub\willard2018a\fig2\data\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3A2B40A-6326-4C29-8047-EFE79741F1FA}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1120" windowWidth="24480" windowHeight="17260" tabRatio="500"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="24480" windowHeight="17265" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Figure 2 Data" sheetId="1" r:id="rId1"/>
@@ -19,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="65">
   <si>
     <t>G5% p values for pairs (p&lt;0.01=synchronous)</t>
   </si>
@@ -155,11 +161,71 @@
   <si>
     <t>Figure #</t>
   </si>
+  <si>
+    <t>N/A(LFP)</t>
+  </si>
+  <si>
+    <t>Ctl % Fractional Beta power</t>
+  </si>
+  <si>
+    <t>G5% Fractional Beta power</t>
+  </si>
+  <si>
+    <t>2G</t>
+  </si>
+  <si>
+    <t>G85% Fractional Beta power</t>
+  </si>
+  <si>
+    <t>G60% Fractional Beta power</t>
+  </si>
+  <si>
+    <t>G30% Fractional Beta power</t>
+  </si>
+  <si>
+    <t>2H</t>
+  </si>
+  <si>
+    <t>2I</t>
+  </si>
+  <si>
+    <t>Ctl PC1</t>
+  </si>
+  <si>
+    <t>Grad PC1</t>
+  </si>
+  <si>
+    <t>A5% PC1</t>
+  </si>
+  <si>
+    <t>PC1</t>
+  </si>
+  <si>
+    <t>Grad %TH</t>
+  </si>
+  <si>
+    <t>A5% %TH</t>
+  </si>
+  <si>
+    <t>FEAT</t>
+  </si>
+  <si>
+    <t>FR</t>
+  </si>
+  <si>
+    <t>IR</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>SYN</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -229,10 +295,18 @@
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="1"/>
+    <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -557,37 +631,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AE362"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:AR362"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AA1" workbookViewId="0">
-      <selection activeCell="AE5" sqref="AE5:AE272"/>
+    <sheetView tabSelected="1" topLeftCell="AD1" workbookViewId="0">
+      <selection activeCell="AK13" sqref="AK13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="12.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="15" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10.625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="12" max="15" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="19" bestFit="1" customWidth="1"/>
-    <col min="23" max="25" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="23" max="25" width="21.875" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.625" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="37.375" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="38.875" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="39" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="40" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="39" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="3" customFormat="1">
+    <row r="1" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>44</v>
       </c>
@@ -681,8 +755,47 @@
       <c r="AE1" s="3" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="2" spans="1:31" s="3" customFormat="1">
+      <c r="AF1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AH1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AI1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AJ1" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="AK1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AL1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AM1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AN1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AO1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AP1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AQ1" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="AR1" s="3" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>38</v>
       </c>
@@ -776,8 +889,44 @@
       <c r="AE2" s="3">
         <v>9</v>
       </c>
-    </row>
-    <row r="3" spans="1:31" s="3" customFormat="1">
+      <c r="AF2" s="3">
+        <v>7</v>
+      </c>
+      <c r="AG2" s="3">
+        <v>6</v>
+      </c>
+      <c r="AH2" s="3">
+        <v>7</v>
+      </c>
+      <c r="AI2" s="3">
+        <v>8</v>
+      </c>
+      <c r="AJ2" s="3">
+        <v>9</v>
+      </c>
+      <c r="AL2" s="3">
+        <v>43</v>
+      </c>
+      <c r="AM2" s="3">
+        <v>7</v>
+      </c>
+      <c r="AN2" s="3">
+        <v>7</v>
+      </c>
+      <c r="AO2" s="3">
+        <v>29</v>
+      </c>
+      <c r="AP2" s="3">
+        <v>29</v>
+      </c>
+      <c r="AQ2" s="3">
+        <v>7</v>
+      </c>
+      <c r="AR2" s="3">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>37</v>
       </c>
@@ -871,8 +1020,23 @@
       <c r="AE3" s="3" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="4" spans="1:31" s="3" customFormat="1">
+      <c r="AF3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AG3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AH3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:44" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>30</v>
       </c>
@@ -966,8 +1130,47 @@
       <c r="AE4" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:31">
+      <c r="AF4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="AG4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="AH4" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="AK4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AL4" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="AM4" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="AN4" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="AO4" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="AP4" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="AQ4" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="AR4" s="3" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B5" s="1">
         <v>100</v>
       </c>
@@ -1058,8 +1261,47 @@
       <c r="AE5">
         <v>0.25213675213675213</v>
       </c>
-    </row>
-    <row r="6" spans="1:31">
+      <c r="AF5">
+        <v>6.5799999999999997E-2</v>
+      </c>
+      <c r="AG5">
+        <v>3.5900000000000001E-2</v>
+      </c>
+      <c r="AH5">
+        <v>8.2000000000000003E-2</v>
+      </c>
+      <c r="AI5">
+        <v>0.13539999999999999</v>
+      </c>
+      <c r="AJ5">
+        <v>7.9399999999999998E-2</v>
+      </c>
+      <c r="AK5" t="s">
+        <v>61</v>
+      </c>
+      <c r="AL5">
+        <v>0.47249999999999998</v>
+      </c>
+      <c r="AM5">
+        <v>0.75696102115700148</v>
+      </c>
+      <c r="AN5">
+        <v>100</v>
+      </c>
+      <c r="AO5">
+        <v>-4.4745331392881817E-2</v>
+      </c>
+      <c r="AP5">
+        <v>17.655644498007536</v>
+      </c>
+      <c r="AQ5">
+        <v>-0.72772875887500643</v>
+      </c>
+      <c r="AR5">
+        <v>4.8969345602702008</v>
+      </c>
+    </row>
+    <row r="6" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B6" s="1">
         <v>100</v>
       </c>
@@ -1150,8 +1392,47 @@
       <c r="AE6">
         <v>3.5612535612535613E-3</v>
       </c>
-    </row>
-    <row r="7" spans="1:31">
+      <c r="AF6">
+        <v>1.61E-2</v>
+      </c>
+      <c r="AG6">
+        <v>5.7299999999999997E-2</v>
+      </c>
+      <c r="AH6">
+        <v>5.6800000000000003E-2</v>
+      </c>
+      <c r="AI6">
+        <v>6.7599999999999993E-2</v>
+      </c>
+      <c r="AJ6">
+        <v>0.1114</v>
+      </c>
+      <c r="AK6" t="s">
+        <v>62</v>
+      </c>
+      <c r="AL6">
+        <v>-0.61839999999999995</v>
+      </c>
+      <c r="AM6">
+        <v>0.97251923557949149</v>
+      </c>
+      <c r="AN6">
+        <v>100</v>
+      </c>
+      <c r="AO6">
+        <v>-0.58721225834224466</v>
+      </c>
+      <c r="AP6">
+        <v>0.52685860928869188</v>
+      </c>
+      <c r="AQ6">
+        <v>-1.4326731776496251</v>
+      </c>
+      <c r="AR6">
+        <v>0.53861583837209315</v>
+      </c>
+    </row>
+    <row r="7" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B7" s="1">
         <v>100</v>
       </c>
@@ -1242,8 +1523,47 @@
       <c r="AE7">
         <v>0.76709401709401703</v>
       </c>
-    </row>
-    <row r="8" spans="1:31">
+      <c r="AF7">
+        <v>0.10290000000000001</v>
+      </c>
+      <c r="AG7">
+        <v>9.0399999999999994E-2</v>
+      </c>
+      <c r="AH7">
+        <v>0.113</v>
+      </c>
+      <c r="AI7">
+        <v>8.4000000000000005E-2</v>
+      </c>
+      <c r="AJ7">
+        <v>8.43E-2</v>
+      </c>
+      <c r="AK7" t="s">
+        <v>63</v>
+      </c>
+      <c r="AL7">
+        <v>-0.61329999999999996</v>
+      </c>
+      <c r="AM7">
+        <v>0.68458445578882621</v>
+      </c>
+      <c r="AN7">
+        <v>100</v>
+      </c>
+      <c r="AO7">
+        <v>-0.93910244227251671</v>
+      </c>
+      <c r="AP7">
+        <v>0.18747521000000009</v>
+      </c>
+      <c r="AQ7">
+        <v>0.49570856407746156</v>
+      </c>
+      <c r="AR7">
+        <v>7.6977440131689043</v>
+      </c>
+    </row>
+    <row r="8" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B8" s="1">
         <v>100</v>
       </c>
@@ -1334,8 +1654,47 @@
       <c r="AE8">
         <v>0.42877492877492879</v>
       </c>
-    </row>
-    <row r="9" spans="1:31">
+      <c r="AF8">
+        <v>7.6700000000000004E-2</v>
+      </c>
+      <c r="AG8">
+        <v>8.6400000000000005E-2</v>
+      </c>
+      <c r="AH8">
+        <v>5.79E-2</v>
+      </c>
+      <c r="AI8">
+        <v>7.0699999999999999E-2</v>
+      </c>
+      <c r="AJ8">
+        <v>7.8799999999999995E-2</v>
+      </c>
+      <c r="AK8" t="s">
+        <v>64</v>
+      </c>
+      <c r="AL8">
+        <v>-0.13519999999999999</v>
+      </c>
+      <c r="AM8">
+        <v>1.4225407279589855</v>
+      </c>
+      <c r="AN8">
+        <v>100</v>
+      </c>
+      <c r="AO8">
+        <v>1.6548469036000761E-2</v>
+      </c>
+      <c r="AP8">
+        <v>2.1144078678333327</v>
+      </c>
+      <c r="AQ8">
+        <v>-0.38687472166717485</v>
+      </c>
+      <c r="AR8">
+        <v>2.1514408332529613</v>
+      </c>
+    </row>
+    <row r="9" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B9" s="1">
         <v>100</v>
       </c>
@@ -1426,8 +1785,41 @@
       <c r="AE9">
         <v>0.19159544159544159</v>
       </c>
-    </row>
-    <row r="10" spans="1:31">
+      <c r="AF9">
+        <v>7.1300000000000002E-2</v>
+      </c>
+      <c r="AG9">
+        <v>7.0599999999999996E-2</v>
+      </c>
+      <c r="AH9">
+        <v>9.9500000000000005E-2</v>
+      </c>
+      <c r="AI9">
+        <v>4.9299999999999997E-2</v>
+      </c>
+      <c r="AJ9">
+        <v>0.1137</v>
+      </c>
+      <c r="AM9">
+        <v>0.40118831555516876</v>
+      </c>
+      <c r="AN9">
+        <v>100</v>
+      </c>
+      <c r="AO9">
+        <v>-1.1365585739669966</v>
+      </c>
+      <c r="AP9">
+        <v>7.3764743014285736</v>
+      </c>
+      <c r="AQ9">
+        <v>-0.33032028079429721</v>
+      </c>
+      <c r="AR9">
+        <v>3.2915089590539739</v>
+      </c>
+    </row>
+    <row r="10" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B10" s="1">
         <v>100</v>
       </c>
@@ -1512,8 +1904,41 @@
       <c r="AE10">
         <v>0.14102564102564102</v>
       </c>
-    </row>
-    <row r="11" spans="1:31">
+      <c r="AF10">
+        <v>0.1057</v>
+      </c>
+      <c r="AG10">
+        <v>6.6199999999999995E-2</v>
+      </c>
+      <c r="AH10">
+        <v>6.5699999999999995E-2</v>
+      </c>
+      <c r="AI10">
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="AJ10">
+        <v>4.6800000000000001E-2</v>
+      </c>
+      <c r="AM10">
+        <v>0.43026488405784463</v>
+      </c>
+      <c r="AN10">
+        <v>100</v>
+      </c>
+      <c r="AO10">
+        <v>-0.90277266126268496</v>
+      </c>
+      <c r="AP10">
+        <v>0.42055814634350602</v>
+      </c>
+      <c r="AQ10">
+        <v>-0.57911349194009198</v>
+      </c>
+      <c r="AR10">
+        <v>7.7308225893126155</v>
+      </c>
+    </row>
+    <row r="11" spans="1:44" x14ac:dyDescent="0.25">
       <c r="B11" s="1">
         <v>100</v>
       </c>
@@ -1598,8 +2023,38 @@
       <c r="AE11">
         <v>1.4245014245014246E-3</v>
       </c>
-    </row>
-    <row r="12" spans="1:31">
+      <c r="AF11">
+        <v>0.1023</v>
+      </c>
+      <c r="AH11">
+        <v>8.5300000000000001E-2</v>
+      </c>
+      <c r="AI11">
+        <v>9.4E-2</v>
+      </c>
+      <c r="AJ11">
+        <v>7.51E-2</v>
+      </c>
+      <c r="AM11">
+        <v>0.86317507641854341</v>
+      </c>
+      <c r="AN11">
+        <v>100</v>
+      </c>
+      <c r="AO11">
+        <v>-3.1309105802673362E-2</v>
+      </c>
+      <c r="AP11">
+        <v>4.4809252299999978</v>
+      </c>
+      <c r="AQ11">
+        <v>-0.6080785378334238</v>
+      </c>
+      <c r="AR11">
+        <v>2.0040828159176662</v>
+      </c>
+    </row>
+    <row r="12" spans="1:44" x14ac:dyDescent="0.25">
       <c r="H12">
         <v>26.326278587231926</v>
       </c>
@@ -1672,8 +2127,20 @@
       <c r="AE12">
         <v>0.34971509971509973</v>
       </c>
-    </row>
-    <row r="13" spans="1:31">
+      <c r="AI12">
+        <v>9.4200000000000006E-2</v>
+      </c>
+      <c r="AJ12">
+        <v>6.5299999999999997E-2</v>
+      </c>
+      <c r="AO12">
+        <v>-0.44613466765296955</v>
+      </c>
+      <c r="AP12">
+        <v>-0.63020281004961709</v>
+      </c>
+    </row>
+    <row r="13" spans="1:44" x14ac:dyDescent="0.25">
       <c r="J13">
         <v>12.089459929887813</v>
       </c>
@@ -1740,8 +2207,17 @@
       <c r="AE13">
         <v>0.51424501424501423</v>
       </c>
-    </row>
-    <row r="14" spans="1:31">
+      <c r="AJ13">
+        <v>7.1199999999999999E-2</v>
+      </c>
+      <c r="AO13">
+        <v>0.47731813178549792</v>
+      </c>
+      <c r="AP13">
+        <v>11.992664108006464</v>
+      </c>
+    </row>
+    <row r="14" spans="1:44" x14ac:dyDescent="0.25">
       <c r="L14">
         <v>12.318184845217566</v>
       </c>
@@ -1802,8 +2278,14 @@
       <c r="AE14">
         <v>0.3368945868945869</v>
       </c>
-    </row>
-    <row r="15" spans="1:31">
+      <c r="AO14">
+        <v>-0.39155543888312394</v>
+      </c>
+      <c r="AP14">
+        <v>24.869636851994645</v>
+      </c>
+    </row>
+    <row r="15" spans="1:44" x14ac:dyDescent="0.25">
       <c r="L15">
         <v>33.545196837459692</v>
       </c>
@@ -1864,8 +2346,14 @@
       <c r="AE15">
         <v>8.5470085470085479E-3</v>
       </c>
-    </row>
-    <row r="16" spans="1:31">
+      <c r="AO15">
+        <v>-1.3742696425238505</v>
+      </c>
+      <c r="AP15">
+        <v>34.442991176612253</v>
+      </c>
+    </row>
+    <row r="16" spans="1:44" x14ac:dyDescent="0.25">
       <c r="L16">
         <v>25.56239291728653</v>
       </c>
@@ -1926,8 +2414,14 @@
       <c r="AE16">
         <v>0.21438746438746437</v>
       </c>
-    </row>
-    <row r="17" spans="12:31">
+      <c r="AO16">
+        <v>-0.67642980886705339</v>
+      </c>
+      <c r="AP16">
+        <v>51.680303766001032</v>
+      </c>
+    </row>
+    <row r="17" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L17">
         <v>38.739429592400349</v>
       </c>
@@ -1988,8 +2482,14 @@
       <c r="AE17">
         <v>0.99643874643874641</v>
       </c>
-    </row>
-    <row r="18" spans="12:31">
+      <c r="AO17">
+        <v>-3.5512741840228651E-2</v>
+      </c>
+      <c r="AP17">
+        <v>29.393349416487645</v>
+      </c>
+    </row>
+    <row r="18" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L18">
         <v>26.204342796449371</v>
       </c>
@@ -2050,8 +2550,14 @@
       <c r="AE18">
         <v>0.33048433048433046</v>
       </c>
-    </row>
-    <row r="19" spans="12:31">
+      <c r="AO18">
+        <v>0.24586175572950153</v>
+      </c>
+      <c r="AP18">
+        <v>13.852703142980921</v>
+      </c>
+    </row>
+    <row r="19" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L19">
         <v>12.674266828884994</v>
       </c>
@@ -2112,8 +2618,14 @@
       <c r="AE19">
         <v>0.93660968660968669</v>
       </c>
-    </row>
-    <row r="20" spans="12:31">
+      <c r="AO19">
+        <v>0.22885011496021856</v>
+      </c>
+      <c r="AP19">
+        <v>32.161916309139229</v>
+      </c>
+    </row>
+    <row r="20" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L20">
         <v>28.840571438828512</v>
       </c>
@@ -2174,8 +2686,14 @@
       <c r="AE20">
         <v>0.95655270655270663</v>
       </c>
-    </row>
-    <row r="21" spans="12:31">
+      <c r="AO20">
+        <v>-8.5771456262959719E-2</v>
+      </c>
+      <c r="AP20">
+        <v>45.717120091605288</v>
+      </c>
+    </row>
+    <row r="21" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L21">
         <v>26.789609327293231</v>
       </c>
@@ -2236,8 +2754,14 @@
       <c r="AE21">
         <v>0.95797720797720798</v>
       </c>
-    </row>
-    <row r="22" spans="12:31">
+      <c r="AO21">
+        <v>0.68446787215510463</v>
+      </c>
+      <c r="AP21">
+        <v>25.595765913119195</v>
+      </c>
+    </row>
+    <row r="22" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L22">
         <v>41.299444096647761</v>
       </c>
@@ -2298,8 +2822,14 @@
       <c r="AE22">
         <v>0.11467236467236466</v>
       </c>
-    </row>
-    <row r="23" spans="12:31">
+      <c r="AO22">
+        <v>-3.0285737973786926E-2</v>
+      </c>
+      <c r="AP22">
+        <v>63.523406571873529</v>
+      </c>
+    </row>
+    <row r="23" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L23">
         <v>4.2434694955567993</v>
       </c>
@@ -2360,8 +2890,14 @@
       <c r="AE23">
         <v>0.41737891737891741</v>
       </c>
-    </row>
-    <row r="24" spans="12:31">
+      <c r="AO23">
+        <v>0.10538673686368692</v>
+      </c>
+      <c r="AP23">
+        <v>61.963398318042792</v>
+      </c>
+    </row>
+    <row r="24" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L24">
         <v>11.673151961569113</v>
       </c>
@@ -2422,8 +2958,14 @@
       <c r="AE24">
         <v>0.7742165242165242</v>
       </c>
-    </row>
-    <row r="25" spans="12:31">
+      <c r="AO24">
+        <v>-0.85855806506237653</v>
+      </c>
+      <c r="AP24">
+        <v>68.336569463007734</v>
+      </c>
+    </row>
+    <row r="25" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L25">
         <v>37.638277991264275</v>
       </c>
@@ -2484,8 +3026,14 @@
       <c r="AE25">
         <v>2.8490028490028491E-3</v>
       </c>
-    </row>
-    <row r="26" spans="12:31">
+      <c r="AO25">
+        <v>0.39351219654459219</v>
+      </c>
+      <c r="AP25">
+        <v>50.496420781133779</v>
+      </c>
+    </row>
+    <row r="26" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L26">
         <v>31.95474685684043</v>
       </c>
@@ -2546,8 +3094,14 @@
       <c r="AE26">
         <v>6.4102564102564109E-3</v>
       </c>
-    </row>
-    <row r="27" spans="12:31">
+      <c r="AO26">
+        <v>0.47291755610634095</v>
+      </c>
+      <c r="AP26">
+        <v>62.772443793909041</v>
+      </c>
+    </row>
+    <row r="27" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L27">
         <v>39.097637291254145</v>
       </c>
@@ -2608,8 +3162,14 @@
       <c r="AE27">
         <v>1.4245014245014246E-3</v>
       </c>
-    </row>
-    <row r="28" spans="12:31">
+      <c r="AO27">
+        <v>0.1205611503910603</v>
+      </c>
+      <c r="AP27">
+        <v>62.715915490966239</v>
+      </c>
+    </row>
+    <row r="28" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L28">
         <v>42.221622456903141</v>
       </c>
@@ -2670,8 +3230,14 @@
       <c r="AE28">
         <v>3.3475783475783477E-2</v>
       </c>
-    </row>
-    <row r="29" spans="12:31">
+      <c r="AO28">
+        <v>0.37111568031920822</v>
+      </c>
+      <c r="AP28">
+        <v>54.324888474515433</v>
+      </c>
+    </row>
+    <row r="29" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L29">
         <v>35.931773447262081</v>
       </c>
@@ -2732,8 +3298,14 @@
       <c r="AE29">
         <v>4.2022792022792022E-2</v>
       </c>
-    </row>
-    <row r="30" spans="12:31">
+      <c r="AO29">
+        <v>0.60270943031392055</v>
+      </c>
+      <c r="AP29">
+        <v>87.406959759175052</v>
+      </c>
+    </row>
+    <row r="30" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L30">
         <v>34.056912865514256</v>
       </c>
@@ -2794,8 +3366,14 @@
       <c r="AE30">
         <v>0.10683760683760683</v>
       </c>
-    </row>
-    <row r="31" spans="12:31">
+      <c r="AO30">
+        <v>0.20195762493650024</v>
+      </c>
+      <c r="AP30">
+        <v>81.669266345316856</v>
+      </c>
+    </row>
+    <row r="31" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L31">
         <v>47.921717486947806</v>
       </c>
@@ -2856,8 +3434,14 @@
       <c r="AE31">
         <v>9.5441595441595445E-2</v>
       </c>
-    </row>
-    <row r="32" spans="12:31">
+      <c r="AO31">
+        <v>-0.66791299254225334</v>
+      </c>
+      <c r="AP31">
+        <v>89.821373966949466</v>
+      </c>
+    </row>
+    <row r="32" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L32">
         <v>31.475399860919165</v>
       </c>
@@ -2918,8 +3502,14 @@
       <c r="AE32">
         <v>2.8490028490028491E-3</v>
       </c>
-    </row>
-    <row r="33" spans="12:31">
+      <c r="AO32">
+        <v>5.0988979390365743E-2</v>
+      </c>
+      <c r="AP32">
+        <v>75.485438544325632</v>
+      </c>
+    </row>
+    <row r="33" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L33">
         <v>9.8394226041814274</v>
       </c>
@@ -2980,8 +3570,14 @@
       <c r="AE33">
         <v>0.21367521367521369</v>
       </c>
-    </row>
-    <row r="34" spans="12:31">
+      <c r="AO33">
+        <v>0.35463028410742081</v>
+      </c>
+      <c r="AP33">
+        <v>93.084378666062776</v>
+      </c>
+    </row>
+    <row r="34" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L34">
         <v>33.821119935962471</v>
       </c>
@@ -3043,7 +3639,7 @@
         <v>1.8518518518518517E-2</v>
       </c>
     </row>
-    <row r="35" spans="12:31">
+    <row r="35" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L35">
         <v>47.240400593863114</v>
       </c>
@@ -3105,7 +3701,7 @@
         <v>1.5669515669515671E-2</v>
       </c>
     </row>
-    <row r="36" spans="12:31">
+    <row r="36" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L36">
         <v>44.927267180103584</v>
       </c>
@@ -3167,7 +3763,7 @@
         <v>1.3532763532763533E-2</v>
       </c>
     </row>
-    <row r="37" spans="12:31">
+    <row r="37" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L37">
         <v>64.923085353207028</v>
       </c>
@@ -3229,7 +3825,7 @@
         <v>0.2727920227920228</v>
       </c>
     </row>
-    <row r="38" spans="12:31">
+    <row r="38" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L38">
         <v>38.732399153981056</v>
       </c>
@@ -3291,7 +3887,7 @@
         <v>0.88746438746438749</v>
       </c>
     </row>
-    <row r="39" spans="12:31">
+    <row r="39" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L39">
         <v>28.80686002100553</v>
       </c>
@@ -3353,7 +3949,7 @@
         <v>0.86111111111111116</v>
       </c>
     </row>
-    <row r="40" spans="12:31">
+    <row r="40" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L40">
         <v>38.446537837355073</v>
       </c>
@@ -3415,7 +4011,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="41" spans="12:31">
+    <row r="41" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L41">
         <v>35.099324478005187</v>
       </c>
@@ -3477,7 +4073,7 @@
         <v>2.136752136752137E-3</v>
       </c>
     </row>
-    <row r="42" spans="12:31">
+    <row r="42" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L42">
         <v>59.158965955490658</v>
       </c>
@@ -3539,7 +4135,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="43" spans="12:31">
+    <row r="43" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L43">
         <v>46.261304776357683</v>
       </c>
@@ -3601,7 +4197,7 @@
         <v>0.11182336182336183</v>
       </c>
     </row>
-    <row r="44" spans="12:31">
+    <row r="44" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L44">
         <v>47.578352599172135</v>
       </c>
@@ -3663,7 +4259,7 @@
         <v>0.8475783475783476</v>
       </c>
     </row>
-    <row r="45" spans="12:31">
+    <row r="45" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L45">
         <v>11.712318138599963</v>
       </c>
@@ -3725,7 +4321,7 @@
         <v>0.10683760683760685</v>
       </c>
     </row>
-    <row r="46" spans="12:31">
+    <row r="46" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L46">
         <v>49.414780417948421</v>
       </c>
@@ -3787,7 +4383,7 @@
         <v>2.3504273504273504E-2</v>
       </c>
     </row>
-    <row r="47" spans="12:31">
+    <row r="47" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L47">
         <v>29.756768146598077</v>
       </c>
@@ -3849,7 +4445,7 @@
         <v>0.37962962962962965</v>
       </c>
     </row>
-    <row r="48" spans="12:31">
+    <row r="48" spans="12:42" x14ac:dyDescent="0.25">
       <c r="L48">
         <v>49.829520642541233</v>
       </c>
@@ -3911,7 +4507,7 @@
         <v>0.56481481481481488</v>
       </c>
     </row>
-    <row r="49" spans="12:31">
+    <row r="49" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L49">
         <v>49.610348979138529</v>
       </c>
@@ -3973,7 +4569,7 @@
         <v>0.86396011396011396</v>
       </c>
     </row>
-    <row r="50" spans="12:31">
+    <row r="50" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L50">
         <v>5.5905633526413157</v>
       </c>
@@ -4035,7 +4631,7 @@
         <v>0.95655270655270652</v>
       </c>
     </row>
-    <row r="51" spans="12:31">
+    <row r="51" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L51">
         <v>4.9566514646457991</v>
       </c>
@@ -4097,7 +4693,7 @@
         <v>0.93945868945868938</v>
       </c>
     </row>
-    <row r="52" spans="12:31">
+    <row r="52" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L52">
         <v>34.492624632359174</v>
       </c>
@@ -4159,7 +4755,7 @@
         <v>0.55698005698005693</v>
       </c>
     </row>
-    <row r="53" spans="12:31">
+    <row r="53" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L53">
         <v>33.612397416221818</v>
       </c>
@@ -4221,7 +4817,7 @@
         <v>0.33119658119658124</v>
       </c>
     </row>
-    <row r="54" spans="12:31">
+    <row r="54" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L54">
         <v>33.544162748304196</v>
       </c>
@@ -4283,7 +4879,7 @@
         <v>4.2735042735042739E-3</v>
       </c>
     </row>
-    <row r="55" spans="12:31">
+    <row r="55" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L55">
         <v>45.891314355486685</v>
       </c>
@@ -4345,7 +4941,7 @@
         <v>0.71509971509971515</v>
       </c>
     </row>
-    <row r="56" spans="12:31">
+    <row r="56" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L56">
         <v>32.268501786016657</v>
       </c>
@@ -4407,7 +5003,7 @@
         <v>0.82692307692307687</v>
       </c>
     </row>
-    <row r="57" spans="12:31">
+    <row r="57" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L57">
         <v>40.547144959130129</v>
       </c>
@@ -4469,7 +5065,7 @@
         <v>1.0683760683760684E-2</v>
       </c>
     </row>
-    <row r="58" spans="12:31">
+    <row r="58" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L58">
         <v>33.853546015797761</v>
       </c>
@@ -4531,7 +5127,7 @@
         <v>2.136752136752137E-3</v>
       </c>
     </row>
-    <row r="59" spans="12:31">
+    <row r="59" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L59">
         <v>43.555432117272836</v>
       </c>
@@ -4593,7 +5189,7 @@
         <v>4.9857549857549865E-3</v>
       </c>
     </row>
-    <row r="60" spans="12:31">
+    <row r="60" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L60">
         <v>45.942817829483495</v>
       </c>
@@ -4655,7 +5251,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="61" spans="12:31">
+    <row r="61" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L61">
         <v>30.23281967711619</v>
       </c>
@@ -4717,7 +5313,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="62" spans="12:31">
+    <row r="62" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L62">
         <v>36.945967082380903</v>
       </c>
@@ -4779,7 +5375,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="63" spans="12:31">
+    <row r="63" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L63">
         <v>14.78259240689458</v>
       </c>
@@ -4841,7 +5437,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="64" spans="12:31">
+    <row r="64" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L64">
         <v>45.535851859360186</v>
       </c>
@@ -4903,7 +5499,7 @@
         <v>2.136752136752137E-3</v>
       </c>
     </row>
-    <row r="65" spans="12:31">
+    <row r="65" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L65">
         <v>31.827797885511988</v>
       </c>
@@ -4965,7 +5561,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="66" spans="12:31">
+    <row r="66" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L66">
         <v>42.360808313191697</v>
       </c>
@@ -5027,7 +5623,7 @@
         <v>3.8461538461538464E-2</v>
       </c>
     </row>
-    <row r="67" spans="12:31">
+    <row r="67" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L67">
         <v>35.448070698657908</v>
       </c>
@@ -5089,7 +5685,7 @@
         <v>1.4957264957264958E-2</v>
       </c>
     </row>
-    <row r="68" spans="12:31">
+    <row r="68" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L68">
         <v>32.274368490203926</v>
       </c>
@@ -5151,7 +5747,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="69" spans="12:31">
+    <row r="69" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L69">
         <v>34.881405097785212</v>
       </c>
@@ -5213,7 +5809,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="70" spans="12:31">
+    <row r="70" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L70">
         <v>27.683170011931697</v>
       </c>
@@ -5275,7 +5871,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="71" spans="12:31">
+    <row r="71" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L71">
         <v>42.748217416978257</v>
       </c>
@@ -5337,7 +5933,7 @@
         <v>2.8490028490028491E-3</v>
       </c>
     </row>
-    <row r="72" spans="12:31">
+    <row r="72" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L72">
         <v>43.745087833031548</v>
       </c>
@@ -5399,7 +5995,7 @@
         <v>0.18874643874643876</v>
       </c>
     </row>
-    <row r="73" spans="12:31">
+    <row r="73" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L73">
         <v>49.742721145669414</v>
       </c>
@@ -5461,7 +6057,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="74" spans="12:31">
+    <row r="74" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L74">
         <v>36.526307550864622</v>
       </c>
@@ -5523,7 +6119,7 @@
         <v>0.46438746438746437</v>
       </c>
     </row>
-    <row r="75" spans="12:31">
+    <row r="75" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L75">
         <v>34.788675469633091</v>
       </c>
@@ -5585,7 +6181,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="76" spans="12:31">
+    <row r="76" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L76">
         <v>38.387333251463176</v>
       </c>
@@ -5647,7 +6243,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="77" spans="12:31">
+    <row r="77" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L77">
         <v>43.406581875703822</v>
       </c>
@@ -5709,7 +6305,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="78" spans="12:31">
+    <row r="78" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L78">
         <v>18.860547216665651</v>
       </c>
@@ -5771,7 +6367,7 @@
         <v>0.99501424501424496</v>
       </c>
     </row>
-    <row r="79" spans="12:31">
+    <row r="79" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L79">
         <v>35.47908852287631</v>
       </c>
@@ -5833,7 +6429,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="80" spans="12:31">
+    <row r="80" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L80">
         <v>46.088048543969187</v>
       </c>
@@ -5895,7 +6491,7 @@
         <v>0.80982905982905984</v>
       </c>
     </row>
-    <row r="81" spans="12:31">
+    <row r="81" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L81">
         <v>51.690404007347922</v>
       </c>
@@ -5957,7 +6553,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="12:31">
+    <row r="82" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L82">
         <v>36.349805289368447</v>
       </c>
@@ -6019,7 +6615,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="83" spans="12:31">
+    <row r="83" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L83">
         <v>18.712869117693913</v>
       </c>
@@ -6081,7 +6677,7 @@
         <v>0.34971509971509973</v>
       </c>
     </row>
-    <row r="84" spans="12:31">
+    <row r="84" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L84">
         <v>61.353601855006758</v>
       </c>
@@ -6143,7 +6739,7 @@
         <v>0.32051282051282048</v>
       </c>
     </row>
-    <row r="85" spans="12:31">
+    <row r="85" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L85">
         <v>7.5186175432863731</v>
       </c>
@@ -6205,7 +6801,7 @@
         <v>4.8433048433048437E-2</v>
       </c>
     </row>
-    <row r="86" spans="12:31">
+    <row r="86" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L86">
         <v>28.446264748363649</v>
       </c>
@@ -6267,7 +6863,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="87" spans="12:31">
+    <row r="87" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L87">
         <v>59.713099196620199</v>
       </c>
@@ -6329,7 +6925,7 @@
         <v>4.9857549857549857E-3</v>
       </c>
     </row>
-    <row r="88" spans="12:31">
+    <row r="88" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L88">
         <v>30.341842932671423</v>
       </c>
@@ -6391,7 +6987,7 @@
         <v>0.1111111111111111</v>
       </c>
     </row>
-    <row r="89" spans="12:31">
+    <row r="89" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L89">
         <v>25.57677158683228</v>
       </c>
@@ -6453,7 +7049,7 @@
         <v>2.564102564102564E-2</v>
       </c>
     </row>
-    <row r="90" spans="12:31">
+    <row r="90" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L90">
         <v>14.522330178657331</v>
       </c>
@@ -6515,7 +7111,7 @@
         <v>0.12179487179487181</v>
       </c>
     </row>
-    <row r="91" spans="12:31">
+    <row r="91" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L91">
         <v>35.047136034064835</v>
       </c>
@@ -6577,7 +7173,7 @@
         <v>0.46438746438746437</v>
       </c>
     </row>
-    <row r="92" spans="12:31">
+    <row r="92" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L92">
         <v>29.310832204478778</v>
       </c>
@@ -6639,7 +7235,7 @@
         <v>0.40811965811965811</v>
       </c>
     </row>
-    <row r="93" spans="12:31">
+    <row r="93" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L93">
         <v>68.342327593042555</v>
       </c>
@@ -6701,7 +7297,7 @@
         <v>0.98433048433048431</v>
       </c>
     </row>
-    <row r="94" spans="12:31">
+    <row r="94" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L94">
         <v>51.373486075926508</v>
       </c>
@@ -6763,7 +7359,7 @@
         <v>0.28917378917378916</v>
       </c>
     </row>
-    <row r="95" spans="12:31">
+    <row r="95" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L95">
         <v>41.020639907175791</v>
       </c>
@@ -6825,7 +7421,7 @@
         <v>3.1339031339031341E-2</v>
       </c>
     </row>
-    <row r="96" spans="12:31">
+    <row r="96" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L96">
         <v>22.130663287814574</v>
       </c>
@@ -6887,7 +7483,7 @@
         <v>0.92165242165242156</v>
       </c>
     </row>
-    <row r="97" spans="12:31">
+    <row r="97" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L97">
         <v>52.752346515375436</v>
       </c>
@@ -6949,7 +7545,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="98" spans="12:31">
+    <row r="98" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L98">
         <v>34.87596128906943</v>
       </c>
@@ -7011,7 +7607,7 @@
         <v>0.18660968660968663</v>
       </c>
     </row>
-    <row r="99" spans="12:31">
+    <row r="99" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L99">
         <v>22.446327166489652</v>
       </c>
@@ -7073,7 +7669,7 @@
         <v>0.96937321937321941</v>
       </c>
     </row>
-    <row r="100" spans="12:31">
+    <row r="100" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L100">
         <v>53.498139535618392</v>
       </c>
@@ -7135,7 +7731,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="12:31">
+    <row r="101" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L101">
         <v>40.508661255608565</v>
       </c>
@@ -7197,7 +7793,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="102" spans="12:31">
+    <row r="102" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L102">
         <v>35.669196903485471</v>
       </c>
@@ -7259,7 +7855,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="103" spans="12:31">
+    <row r="103" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L103">
         <v>51.525602795681536</v>
       </c>
@@ -7321,7 +7917,7 @@
         <v>0.93945868945868949</v>
       </c>
     </row>
-    <row r="104" spans="12:31">
+    <row r="104" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L104">
         <v>50.96577747017006</v>
       </c>
@@ -7383,7 +7979,7 @@
         <v>9.5441595441595445E-2</v>
       </c>
     </row>
-    <row r="105" spans="12:31">
+    <row r="105" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L105">
         <v>24.755905192302983</v>
       </c>
@@ -7445,7 +8041,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="106" spans="12:31">
+    <row r="106" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L106">
         <v>19.090049327128607</v>
       </c>
@@ -7507,7 +8103,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="107" spans="12:31">
+    <row r="107" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L107">
         <v>35.617718992188486</v>
       </c>
@@ -7569,7 +8165,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="108" spans="12:31">
+    <row r="108" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L108">
         <v>47.674449936389998</v>
       </c>
@@ -7631,7 +8227,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="109" spans="12:31">
+    <row r="109" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L109">
         <v>48.419901739718718</v>
       </c>
@@ -7693,7 +8289,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="110" spans="12:31">
+    <row r="110" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L110">
         <v>46.085758524536054</v>
       </c>
@@ -7755,7 +8351,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="111" spans="12:31">
+    <row r="111" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L111">
         <v>13.917835613377822</v>
       </c>
@@ -7817,7 +8413,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="112" spans="12:31">
+    <row r="112" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L112">
         <v>42.683208764278938</v>
       </c>
@@ -7879,7 +8475,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="113" spans="12:31">
+    <row r="113" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L113">
         <v>21.557216104973207</v>
       </c>
@@ -7941,7 +8537,7 @@
         <v>0.78133903133903138</v>
       </c>
     </row>
-    <row r="114" spans="12:31">
+    <row r="114" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L114">
         <v>19.012494945552703</v>
       </c>
@@ -8003,7 +8599,7 @@
         <v>0.32193732193732194</v>
       </c>
     </row>
-    <row r="115" spans="12:31">
+    <row r="115" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L115">
         <v>66.76103953123598</v>
       </c>
@@ -8065,7 +8661,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="116" spans="12:31">
+    <row r="116" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L116">
         <v>21.303209463175339</v>
       </c>
@@ -8127,7 +8723,7 @@
         <v>3.2763532763532763E-2</v>
       </c>
     </row>
-    <row r="117" spans="12:31">
+    <row r="117" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L117">
         <v>30.036551110909802</v>
       </c>
@@ -8189,7 +8785,7 @@
         <v>0.52564102564102566</v>
       </c>
     </row>
-    <row r="118" spans="12:31">
+    <row r="118" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L118">
         <v>69.59737577167418</v>
       </c>
@@ -8251,7 +8847,7 @@
         <v>0.97507122507122501</v>
       </c>
     </row>
-    <row r="119" spans="12:31">
+    <row r="119" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L119">
         <v>50.381312120412787</v>
       </c>
@@ -8313,7 +8909,7 @@
         <v>0.18091168091168092</v>
       </c>
     </row>
-    <row r="120" spans="12:31">
+    <row r="120" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L120">
         <v>37.177615481260631</v>
       </c>
@@ -8375,7 +8971,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="121" spans="12:31">
+    <row r="121" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L121">
         <v>50.70728015973355</v>
       </c>
@@ -8437,7 +9033,7 @@
         <v>6.41025641025641E-3</v>
       </c>
     </row>
-    <row r="122" spans="12:31">
+    <row r="122" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L122">
         <v>46.916244316403201</v>
       </c>
@@ -8499,7 +9095,7 @@
         <v>8.5470085470085479E-3</v>
       </c>
     </row>
-    <row r="123" spans="12:31">
+    <row r="123" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L123">
         <v>59.069142506546676</v>
       </c>
@@ -8561,7 +9157,7 @@
         <v>1.4957264957264958E-2</v>
       </c>
     </row>
-    <row r="124" spans="12:31">
+    <row r="124" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L124">
         <v>47.238738343797806</v>
       </c>
@@ -8623,7 +9219,7 @@
         <v>0.27849002849002846</v>
       </c>
     </row>
-    <row r="125" spans="12:31">
+    <row r="125" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L125">
         <v>51.860764920781165</v>
       </c>
@@ -8685,7 +9281,7 @@
         <v>0.90598290598290598</v>
       </c>
     </row>
-    <row r="126" spans="12:31">
+    <row r="126" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L126">
         <v>36.406858156116066</v>
       </c>
@@ -8747,7 +9343,7 @@
         <v>0.68660968660968658</v>
       </c>
     </row>
-    <row r="127" spans="12:31">
+    <row r="127" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L127">
         <v>31.447284747909098</v>
       </c>
@@ -8809,7 +9405,7 @@
         <v>0.24430199430199431</v>
       </c>
     </row>
-    <row r="128" spans="12:31">
+    <row r="128" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L128">
         <v>45.78084590867801</v>
       </c>
@@ -8871,7 +9467,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="12:31">
+    <row r="129" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L129">
         <v>49.423937273898169</v>
       </c>
@@ -8933,7 +9529,7 @@
         <v>0.89601139601139601</v>
       </c>
     </row>
-    <row r="130" spans="12:31">
+    <row r="130" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L130">
         <v>5.3646236978875486</v>
       </c>
@@ -8995,7 +9591,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="12:31">
+    <row r="131" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L131">
         <v>4.0595492436218317</v>
       </c>
@@ -9057,7 +9653,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="132" spans="12:31">
+    <row r="132" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L132">
         <v>2.3214971468820762</v>
       </c>
@@ -9119,7 +9715,7 @@
         <v>0.21011396011396011</v>
       </c>
     </row>
-    <row r="133" spans="12:31">
+    <row r="133" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L133">
         <v>31.825392103552694</v>
       </c>
@@ -9181,7 +9777,7 @@
         <v>0.12749287749287749</v>
       </c>
     </row>
-    <row r="134" spans="12:31">
+    <row r="134" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L134">
         <v>17.494616675427569</v>
       </c>
@@ -9243,7 +9839,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="12:31">
+    <row r="135" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L135">
         <v>26.079393182410517</v>
       </c>
@@ -9305,7 +9901,7 @@
         <v>0.27706552706552706</v>
       </c>
     </row>
-    <row r="136" spans="12:31">
+    <row r="136" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L136">
         <v>32.503270301772083</v>
       </c>
@@ -9367,7 +9963,7 @@
         <v>0.11894586894586895</v>
       </c>
     </row>
-    <row r="137" spans="12:31">
+    <row r="137" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L137">
         <v>36.847575935611204</v>
       </c>
@@ -9429,7 +10025,7 @@
         <v>0.17877492877492879</v>
       </c>
     </row>
-    <row r="138" spans="12:31">
+    <row r="138" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L138">
         <v>49.126045935781434</v>
       </c>
@@ -9491,7 +10087,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="139" spans="12:31">
+    <row r="139" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L139">
         <v>23.477213260171922</v>
       </c>
@@ -9553,7 +10149,7 @@
         <v>0.21652421652421652</v>
       </c>
     </row>
-    <row r="140" spans="12:31">
+    <row r="140" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L140">
         <v>27.786995769520754</v>
       </c>
@@ -9615,7 +10211,7 @@
         <v>0.23504273504273504</v>
       </c>
     </row>
-    <row r="141" spans="12:31">
+    <row r="141" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L141">
         <v>45.912423294809692</v>
       </c>
@@ -9677,7 +10273,7 @@
         <v>0.3354700854700855</v>
       </c>
     </row>
-    <row r="142" spans="12:31">
+    <row r="142" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L142">
         <v>2.7543022275795583</v>
       </c>
@@ -9739,7 +10335,7 @@
         <v>0.18874643874643876</v>
       </c>
     </row>
-    <row r="143" spans="12:31">
+    <row r="143" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L143">
         <v>24.825176596229049</v>
       </c>
@@ -9801,7 +10397,7 @@
         <v>0.38532763532763536</v>
       </c>
     </row>
-    <row r="144" spans="12:31">
+    <row r="144" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L144">
         <v>27.429475035972668</v>
       </c>
@@ -9863,7 +10459,7 @@
         <v>0.97649572649572647</v>
       </c>
     </row>
-    <row r="145" spans="12:31">
+    <row r="145" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L145">
         <v>43.398802672410035</v>
       </c>
@@ -9925,7 +10521,7 @@
         <v>0.95156695156695159</v>
       </c>
     </row>
-    <row r="146" spans="12:31">
+    <row r="146" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L146">
         <v>43.366470524711296</v>
       </c>
@@ -9987,7 +10583,7 @@
         <v>0.99928774928774922</v>
       </c>
     </row>
-    <row r="147" spans="12:31">
+    <row r="147" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L147">
         <v>30.056477501455728</v>
       </c>
@@ -10049,7 +10645,7 @@
         <v>0.61253561253561251</v>
       </c>
     </row>
-    <row r="148" spans="12:31">
+    <row r="148" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L148">
         <v>29.239486462593632</v>
       </c>
@@ -10111,7 +10707,7 @@
         <v>0.13746438746438747</v>
       </c>
     </row>
-    <row r="149" spans="12:31">
+    <row r="149" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L149">
         <v>18.205902851821609</v>
       </c>
@@ -10173,7 +10769,7 @@
         <v>0.24145299145299143</v>
       </c>
     </row>
-    <row r="150" spans="12:31">
+    <row r="150" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L150">
         <v>16.842865228510927</v>
       </c>
@@ -10235,7 +10831,7 @@
         <v>0.53490028490028485</v>
       </c>
     </row>
-    <row r="151" spans="12:31">
+    <row r="151" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L151">
         <v>36.972828424888043</v>
       </c>
@@ -10297,7 +10893,7 @@
         <v>1.1396011396011397E-2</v>
       </c>
     </row>
-    <row r="152" spans="12:31">
+    <row r="152" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L152">
         <v>36.356713153933484</v>
       </c>
@@ -10359,7 +10955,7 @@
         <v>0.68304843304843299</v>
       </c>
     </row>
-    <row r="153" spans="12:31">
+    <row r="153" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L153">
         <v>14.744623063588572</v>
       </c>
@@ -10421,7 +11017,7 @@
         <v>0.57977207977207978</v>
       </c>
     </row>
-    <row r="154" spans="12:31">
+    <row r="154" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L154">
         <v>13.371129658237303</v>
       </c>
@@ -10483,7 +11079,7 @@
         <v>0.25356125356125359</v>
       </c>
     </row>
-    <row r="155" spans="12:31">
+    <row r="155" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L155">
         <v>14.521195021270966</v>
       </c>
@@ -10545,7 +11141,7 @@
         <v>8.11965811965812E-2</v>
       </c>
     </row>
-    <row r="156" spans="12:31">
+    <row r="156" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L156">
         <v>41.14738433452424</v>
       </c>
@@ -10607,7 +11203,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="157" spans="12:31">
+    <row r="157" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L157">
         <v>39.386072771248429</v>
       </c>
@@ -10669,7 +11265,7 @@
         <v>0.99643874643874641</v>
       </c>
     </row>
-    <row r="158" spans="12:31">
+    <row r="158" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L158">
         <v>33.224901296093869</v>
       </c>
@@ -10731,7 +11327,7 @@
         <v>0.65099715099715105</v>
       </c>
     </row>
-    <row r="159" spans="12:31">
+    <row r="159" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L159">
         <v>13.663452247417077</v>
       </c>
@@ -10793,7 +11389,7 @@
         <v>2.136752136752137E-3</v>
       </c>
     </row>
-    <row r="160" spans="12:31">
+    <row r="160" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L160">
         <v>18.567064032948757</v>
       </c>
@@ -10855,7 +11451,7 @@
         <v>2.9914529914529916E-2</v>
       </c>
     </row>
-    <row r="161" spans="12:31">
+    <row r="161" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L161">
         <v>43.022959520448175</v>
       </c>
@@ -10917,7 +11513,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="162" spans="12:31">
+    <row r="162" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L162">
         <v>42.665286460301928</v>
       </c>
@@ -10979,7 +11575,7 @@
         <v>0.97507122507122501</v>
       </c>
     </row>
-    <row r="163" spans="12:31">
+    <row r="163" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L163">
         <v>37.080295110886773</v>
       </c>
@@ -11041,7 +11637,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="164" spans="12:31">
+    <row r="164" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L164">
         <v>44.177383852540373</v>
       </c>
@@ -11103,7 +11699,7 @@
         <v>0.4665242165242165</v>
       </c>
     </row>
-    <row r="165" spans="12:31">
+    <row r="165" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L165">
         <v>16.302154989377243</v>
       </c>
@@ -11165,7 +11761,7 @@
         <v>0.68233618233618243</v>
       </c>
     </row>
-    <row r="166" spans="12:31">
+    <row r="166" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L166">
         <v>41.736567792880315</v>
       </c>
@@ -11227,7 +11823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="167" spans="12:31">
+    <row r="167" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L167">
         <v>31.324961788392894</v>
       </c>
@@ -11289,7 +11885,7 @@
         <v>0.32264957264957267</v>
       </c>
     </row>
-    <row r="168" spans="12:31">
+    <row r="168" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L168">
         <v>13.046577887074982</v>
       </c>
@@ -11351,7 +11947,7 @@
         <v>0.20299145299145299</v>
       </c>
     </row>
-    <row r="169" spans="12:31">
+    <row r="169" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L169">
         <v>46.073728956513634</v>
       </c>
@@ -11413,7 +12009,7 @@
         <v>0.18518518518518517</v>
       </c>
     </row>
-    <row r="170" spans="12:31">
+    <row r="170" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L170">
         <v>42.62722668957182</v>
       </c>
@@ -11475,7 +12071,7 @@
         <v>0.88532763532763536</v>
       </c>
     </row>
-    <row r="171" spans="12:31">
+    <row r="171" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L171">
         <v>26.982108515155456</v>
       </c>
@@ -11537,7 +12133,7 @@
         <v>0.70512820512820507</v>
       </c>
     </row>
-    <row r="172" spans="12:31">
+    <row r="172" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L172">
         <v>14.81209428624474</v>
       </c>
@@ -11599,7 +12195,7 @@
         <v>0.97222222222222221</v>
       </c>
     </row>
-    <row r="173" spans="12:31">
+    <row r="173" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L173">
         <v>13.592947737461381</v>
       </c>
@@ -11661,7 +12257,7 @@
         <v>0.98789173789173779</v>
       </c>
     </row>
-    <row r="174" spans="12:31">
+    <row r="174" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L174">
         <v>40.557180203514442</v>
       </c>
@@ -11723,7 +12319,7 @@
         <v>0.99572649572649574</v>
       </c>
     </row>
-    <row r="175" spans="12:31">
+    <row r="175" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L175">
         <v>13.165786342495799</v>
       </c>
@@ -11785,7 +12381,7 @@
         <v>0.3368945868945869</v>
       </c>
     </row>
-    <row r="176" spans="12:31">
+    <row r="176" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L176">
         <v>37.799959093648432</v>
       </c>
@@ -11847,7 +12443,7 @@
         <v>4.7008547008547008E-2</v>
       </c>
     </row>
-    <row r="177" spans="12:31">
+    <row r="177" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L177">
         <v>43.852414785571654</v>
       </c>
@@ -11909,7 +12505,7 @@
         <v>0.95868945868945865</v>
       </c>
     </row>
-    <row r="178" spans="12:31">
+    <row r="178" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L178">
         <v>51.013867599216987</v>
       </c>
@@ -11971,7 +12567,7 @@
         <v>0.46794871794871795</v>
       </c>
     </row>
-    <row r="179" spans="12:31">
+    <row r="179" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L179">
         <v>50.364218397734803</v>
       </c>
@@ -12033,7 +12629,7 @@
         <v>0.51139601139601143</v>
       </c>
     </row>
-    <row r="180" spans="12:31">
+    <row r="180" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L180">
         <v>43.690860021197715</v>
       </c>
@@ -12095,7 +12691,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="181" spans="12:31">
+    <row r="181" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L181">
         <v>13.369117018138178</v>
       </c>
@@ -12157,7 +12753,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="182" spans="12:31">
+    <row r="182" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L182">
         <v>34.394366007091676</v>
       </c>
@@ -12219,7 +12815,7 @@
         <v>0.9850427350427351</v>
       </c>
     </row>
-    <row r="183" spans="12:31">
+    <row r="183" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L183">
         <v>47.144604039323013</v>
       </c>
@@ -12281,7 +12877,7 @@
         <v>0.95085470085470081</v>
       </c>
     </row>
-    <row r="184" spans="12:31">
+    <row r="184" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L184">
         <v>20.842774385269536</v>
       </c>
@@ -12343,7 +12939,7 @@
         <v>0.94159544159544151</v>
       </c>
     </row>
-    <row r="185" spans="12:31">
+    <row r="185" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L185">
         <v>94.093780891308796</v>
       </c>
@@ -12405,7 +13001,7 @@
         <v>0.89245014245014243</v>
       </c>
     </row>
-    <row r="186" spans="12:31">
+    <row r="186" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L186">
         <v>26.101342477335248</v>
       </c>
@@ -12467,7 +13063,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="187" spans="12:31">
+    <row r="187" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L187">
         <v>17.633356971530151</v>
       </c>
@@ -12529,7 +13125,7 @@
         <v>0.69017094017094016</v>
       </c>
     </row>
-    <row r="188" spans="12:31">
+    <row r="188" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L188">
         <v>10.251790691675001</v>
       </c>
@@ -12591,7 +13187,7 @@
         <v>8.68945868945869E-2</v>
       </c>
     </row>
-    <row r="189" spans="12:31">
+    <row r="189" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L189">
         <v>63.771608493739222</v>
       </c>
@@ -12653,7 +13249,7 @@
         <v>0.28632478632478631</v>
       </c>
     </row>
-    <row r="190" spans="12:31">
+    <row r="190" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L190">
         <v>41.280868719878661</v>
       </c>
@@ -12715,7 +13311,7 @@
         <v>0.83190883190883191</v>
       </c>
     </row>
-    <row r="191" spans="12:31">
+    <row r="191" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L191">
         <v>74.14113333542555</v>
       </c>
@@ -12777,7 +13373,7 @@
         <v>0.69871794871794868</v>
       </c>
     </row>
-    <row r="192" spans="12:31">
+    <row r="192" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L192">
         <v>39.117102772508034</v>
       </c>
@@ -12839,7 +13435,7 @@
         <v>0.50498575498575504</v>
       </c>
     </row>
-    <row r="193" spans="12:31">
+    <row r="193" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L193">
         <v>38.630194922177488</v>
       </c>
@@ -12901,7 +13497,7 @@
         <v>0.40028490028490027</v>
       </c>
     </row>
-    <row r="194" spans="12:31">
+    <row r="194" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L194">
         <v>73.507891375671846</v>
       </c>
@@ -12963,7 +13559,7 @@
         <v>5.128205128205128E-2</v>
       </c>
     </row>
-    <row r="195" spans="12:31">
+    <row r="195" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L195">
         <v>50.097369777738628</v>
       </c>
@@ -13025,7 +13621,7 @@
         <v>0.81837606837606836</v>
       </c>
     </row>
-    <row r="196" spans="12:31">
+    <row r="196" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L196">
         <v>14.118016906886309</v>
       </c>
@@ -13087,7 +13683,7 @@
         <v>0.59188034188034189</v>
       </c>
     </row>
-    <row r="197" spans="12:31">
+    <row r="197" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L197">
         <v>56.766101551313149</v>
       </c>
@@ -13149,7 +13745,7 @@
         <v>0.51139601139601143</v>
       </c>
     </row>
-    <row r="198" spans="12:31">
+    <row r="198" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L198">
         <v>25.279830025675462</v>
       </c>
@@ -13211,7 +13807,7 @@
         <v>0.74786324786324787</v>
       </c>
     </row>
-    <row r="199" spans="12:31">
+    <row r="199" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L199">
         <v>24.862814212571756</v>
       </c>
@@ -13273,7 +13869,7 @@
         <v>0.32264957264957261</v>
       </c>
     </row>
-    <row r="200" spans="12:31">
+    <row r="200" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L200">
         <v>11.545647975466609</v>
       </c>
@@ -13335,7 +13931,7 @@
         <v>0.65811965811965811</v>
       </c>
     </row>
-    <row r="201" spans="12:31">
+    <row r="201" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L201">
         <v>63.589981770090681</v>
       </c>
@@ -13397,7 +13993,7 @@
         <v>0.61680911680911676</v>
       </c>
     </row>
-    <row r="202" spans="12:31">
+    <row r="202" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L202">
         <v>68.298977993740223</v>
       </c>
@@ -13459,7 +14055,7 @@
         <v>0.82193732193732194</v>
       </c>
     </row>
-    <row r="203" spans="12:31">
+    <row r="203" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L203">
         <v>27.594830709062958</v>
       </c>
@@ -13521,7 +14117,7 @@
         <v>0.82834757834757833</v>
       </c>
     </row>
-    <row r="204" spans="12:31">
+    <row r="204" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L204">
         <v>30.55549637977618</v>
       </c>
@@ -13583,7 +14179,7 @@
         <v>0.87820512820512819</v>
       </c>
     </row>
-    <row r="205" spans="12:31">
+    <row r="205" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L205">
         <v>60.223533990755143</v>
       </c>
@@ -13645,7 +14241,7 @@
         <v>0.72863247863247871</v>
       </c>
     </row>
-    <row r="206" spans="12:31">
+    <row r="206" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L206">
         <v>37.32782518100737</v>
       </c>
@@ -13707,7 +14303,7 @@
         <v>0.2378917378917379</v>
       </c>
     </row>
-    <row r="207" spans="12:31">
+    <row r="207" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L207">
         <v>13.499508447931271</v>
       </c>
@@ -13769,7 +14365,7 @@
         <v>2.1367521367521368E-2</v>
       </c>
     </row>
-    <row r="208" spans="12:31">
+    <row r="208" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L208">
         <v>16.96616343590798</v>
       </c>
@@ -13831,7 +14427,7 @@
         <v>0.6951566951566952</v>
       </c>
     </row>
-    <row r="209" spans="12:31">
+    <row r="209" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L209">
         <v>26.572207391455716</v>
       </c>
@@ -13893,7 +14489,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="210" spans="12:31">
+    <row r="210" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L210">
         <v>28.811216114861832</v>
       </c>
@@ -13955,7 +14551,7 @@
         <v>3.5612535612535613E-3</v>
       </c>
     </row>
-    <row r="211" spans="12:31">
+    <row r="211" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L211">
         <v>4.4221582504049115</v>
       </c>
@@ -14017,7 +14613,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="212" spans="12:31">
+    <row r="212" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L212">
         <v>22.686114911172751</v>
       </c>
@@ -14079,7 +14675,7 @@
         <v>0.16951566951566951</v>
       </c>
     </row>
-    <row r="213" spans="12:31">
+    <row r="213" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L213">
         <v>60.95802874970434</v>
       </c>
@@ -14141,7 +14737,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="214" spans="12:31">
+    <row r="214" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L214">
         <v>30.309874450463422</v>
       </c>
@@ -14203,7 +14799,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="215" spans="12:31">
+    <row r="215" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L215">
         <v>58.969984426003059</v>
       </c>
@@ -14265,7 +14861,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="216" spans="12:31">
+    <row r="216" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L216">
         <v>28.948199756006144</v>
       </c>
@@ -14327,7 +14923,7 @@
         <v>2.8490028490028491E-2</v>
       </c>
     </row>
-    <row r="217" spans="12:31">
+    <row r="217" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L217">
         <v>23.103639244682309</v>
       </c>
@@ -14389,7 +14985,7 @@
         <v>2.8490028490028491E-3</v>
       </c>
     </row>
-    <row r="218" spans="12:31">
+    <row r="218" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L218">
         <v>64.078514587723333</v>
       </c>
@@ -14451,7 +15047,7 @@
         <v>2.9202279202279201E-2</v>
       </c>
     </row>
-    <row r="219" spans="12:31">
+    <row r="219" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L219">
         <v>29.518525304355588</v>
       </c>
@@ -14513,7 +15109,7 @@
         <v>0.26566951566951569</v>
       </c>
     </row>
-    <row r="220" spans="12:31">
+    <row r="220" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L220">
         <v>26.384064530971376</v>
       </c>
@@ -14575,7 +15171,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="221" spans="12:31">
+    <row r="221" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L221">
         <v>28.62506156897857</v>
       </c>
@@ -14637,7 +15233,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="222" spans="12:31">
+    <row r="222" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L222">
         <v>63.371653814342594</v>
       </c>
@@ -14699,7 +15295,7 @@
         <v>7.3361823361823369E-2</v>
       </c>
     </row>
-    <row r="223" spans="12:31">
+    <row r="223" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L223">
         <v>32.035027973578636</v>
       </c>
@@ -14761,7 +15357,7 @@
         <v>0.4358974358974359</v>
       </c>
     </row>
-    <row r="224" spans="12:31">
+    <row r="224" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L224">
         <v>19.145329129100013</v>
       </c>
@@ -14823,7 +15419,7 @@
         <v>0.10327635327635327</v>
       </c>
     </row>
-    <row r="225" spans="12:31">
+    <row r="225" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L225">
         <v>11.237780703330566</v>
       </c>
@@ -14885,7 +15481,7 @@
         <v>0.11182336182336182</v>
       </c>
     </row>
-    <row r="226" spans="12:31">
+    <row r="226" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L226">
         <v>22.845889710246023</v>
       </c>
@@ -14947,7 +15543,7 @@
         <v>0.16025641025641024</v>
       </c>
     </row>
-    <row r="227" spans="12:31">
+    <row r="227" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L227">
         <v>32.508091812869964</v>
       </c>
@@ -15009,7 +15605,7 @@
         <v>1.9230769230769232E-2</v>
       </c>
     </row>
-    <row r="228" spans="12:31">
+    <row r="228" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L228">
         <v>46.206872326877047</v>
       </c>
@@ -15071,7 +15667,7 @@
         <v>0.88960113960113962</v>
       </c>
     </row>
-    <row r="229" spans="12:31">
+    <row r="229" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L229">
         <v>21.77833096934781</v>
       </c>
@@ -15133,7 +15729,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="230" spans="12:31">
+    <row r="230" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L230">
         <v>40.711622280056808</v>
       </c>
@@ -15195,7 +15791,7 @@
         <v>0.12250712250712251</v>
       </c>
     </row>
-    <row r="231" spans="12:31">
+    <row r="231" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L231">
         <v>44.23335134108946</v>
       </c>
@@ -15257,7 +15853,7 @@
         <v>0.96225071225071224</v>
       </c>
     </row>
-    <row r="232" spans="12:31">
+    <row r="232" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L232">
         <v>47.9577698444837</v>
       </c>
@@ -15319,7 +15915,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="233" spans="12:31">
+    <row r="233" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L233">
         <v>42.239535197484194</v>
       </c>
@@ -15381,7 +15977,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="234" spans="12:31">
+    <row r="234" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L234">
         <v>6.6962389273148197</v>
       </c>
@@ -15443,7 +16039,7 @@
         <v>2.7777777777777776E-2</v>
       </c>
     </row>
-    <row r="235" spans="12:31">
+    <row r="235" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L235">
         <v>44.092488485474547</v>
       </c>
@@ -15505,7 +16101,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="236" spans="12:31">
+    <row r="236" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L236">
         <v>20.494592006616127</v>
       </c>
@@ -15567,7 +16163,7 @@
         <v>3.2763532763532763E-2</v>
       </c>
     </row>
-    <row r="237" spans="12:31">
+    <row r="237" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L237">
         <v>6.440954591129878</v>
       </c>
@@ -15629,7 +16225,7 @@
         <v>0.38247863247863245</v>
       </c>
     </row>
-    <row r="238" spans="12:31">
+    <row r="238" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L238">
         <v>6.3746060218585816</v>
       </c>
@@ -15691,7 +16287,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="239" spans="12:31">
+    <row r="239" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L239">
         <v>43.603415195536407</v>
       </c>
@@ -15753,7 +16349,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="240" spans="12:31">
+    <row r="240" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L240">
         <v>22.885945624496014</v>
       </c>
@@ -15815,7 +16411,7 @@
         <v>2.9202279202279205E-2</v>
       </c>
     </row>
-    <row r="241" spans="12:31">
+    <row r="241" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L241">
         <v>44.391454694912191</v>
       </c>
@@ -15877,7 +16473,7 @@
         <v>0.79843304843304841</v>
       </c>
     </row>
-    <row r="242" spans="12:31">
+    <row r="242" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L242">
         <v>22.045857480153895</v>
       </c>
@@ -15939,7 +16535,7 @@
         <v>2.136752136752137E-3</v>
       </c>
     </row>
-    <row r="243" spans="12:31">
+    <row r="243" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L243">
         <v>44.683351416386088</v>
       </c>
@@ -16001,7 +16597,7 @@
         <v>0.59330484330484334</v>
       </c>
     </row>
-    <row r="244" spans="12:31">
+    <row r="244" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L244">
         <v>24.258369147517044</v>
       </c>
@@ -16063,7 +16659,7 @@
         <v>0.20441595441595442</v>
       </c>
     </row>
-    <row r="245" spans="12:31">
+    <row r="245" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L245">
         <v>47.846245207308463</v>
       </c>
@@ -16125,7 +16721,7 @@
         <v>4.9857549857549865E-3</v>
       </c>
     </row>
-    <row r="246" spans="12:31">
+    <row r="246" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L246">
         <v>45.578669761956682</v>
       </c>
@@ -16187,7 +16783,7 @@
         <v>3.5612535612535613E-3</v>
       </c>
     </row>
-    <row r="247" spans="12:31">
+    <row r="247" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L247">
         <v>47.929859920406166</v>
       </c>
@@ -16249,7 +16845,7 @@
         <v>0.4878917378917379</v>
       </c>
     </row>
-    <row r="248" spans="12:31">
+    <row r="248" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L248">
         <v>28.106133445863385</v>
       </c>
@@ -16311,7 +16907,7 @@
         <v>0.85754985754985746</v>
       </c>
     </row>
-    <row r="249" spans="12:31">
+    <row r="249" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L249">
         <v>50.203646330934092</v>
       </c>
@@ -16373,7 +16969,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="250" spans="12:31">
+    <row r="250" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L250">
         <v>45.835562650169607</v>
       </c>
@@ -16432,7 +17028,7 @@
         <v>0.77279202279202275</v>
       </c>
     </row>
-    <row r="251" spans="12:31">
+    <row r="251" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L251">
         <v>22.436510360257845</v>
       </c>
@@ -16491,7 +17087,7 @@
         <v>0.36039886039886038</v>
       </c>
     </row>
-    <row r="252" spans="12:31">
+    <row r="252" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L252">
         <v>23.711756267058213</v>
       </c>
@@ -16550,7 +17146,7 @@
         <v>0.31837606837606836</v>
       </c>
     </row>
-    <row r="253" spans="12:31">
+    <row r="253" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L253">
         <v>23.27670761446991</v>
       </c>
@@ -16609,7 +17205,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="254" spans="12:31">
+    <row r="254" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L254">
         <v>25.44915196801735</v>
       </c>
@@ -16668,7 +17264,7 @@
         <v>0.93447293447293445</v>
       </c>
     </row>
-    <row r="255" spans="12:31">
+    <row r="255" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L255">
         <v>45.980383162394752</v>
       </c>
@@ -16727,7 +17323,7 @@
         <v>6.41025641025641E-3</v>
       </c>
     </row>
-    <row r="256" spans="12:31">
+    <row r="256" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L256">
         <v>35.27773994483465</v>
       </c>
@@ -16786,7 +17382,7 @@
         <v>5.128205128205128E-2</v>
       </c>
     </row>
-    <row r="257" spans="12:31">
+    <row r="257" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L257">
         <v>38.041350291083653</v>
       </c>
@@ -16845,7 +17441,7 @@
         <v>0.99002849002849003</v>
       </c>
     </row>
-    <row r="258" spans="12:31">
+    <row r="258" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L258">
         <v>49.175808859982126</v>
       </c>
@@ -16904,7 +17500,7 @@
         <v>0.92806267806267806</v>
       </c>
     </row>
-    <row r="259" spans="12:31">
+    <row r="259" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L259">
         <v>27.572188344976784</v>
       </c>
@@ -16963,7 +17559,7 @@
         <v>0.88532763532763536</v>
       </c>
     </row>
-    <row r="260" spans="12:31">
+    <row r="260" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L260">
         <v>41.392451860692589</v>
       </c>
@@ -17022,7 +17618,7 @@
         <v>0.71794871794871795</v>
       </c>
     </row>
-    <row r="261" spans="12:31">
+    <row r="261" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L261">
         <v>36.388218442601271</v>
       </c>
@@ -17081,7 +17677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="262" spans="12:31">
+    <row r="262" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L262">
         <v>40.689264900169526</v>
       </c>
@@ -17140,7 +17736,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="263" spans="12:31">
+    <row r="263" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L263">
         <v>54.152223018145079</v>
       </c>
@@ -17199,7 +17795,7 @@
         <v>0.9850427350427351</v>
       </c>
     </row>
-    <row r="264" spans="12:31">
+    <row r="264" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L264">
         <v>42.967149738217202</v>
       </c>
@@ -17258,7 +17854,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="265" spans="12:31">
+    <row r="265" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L265">
         <v>67.081202058120908</v>
       </c>
@@ -17317,7 +17913,7 @@
         <v>0.71153846153846145</v>
       </c>
     </row>
-    <row r="266" spans="12:31">
+    <row r="266" spans="12:31" x14ac:dyDescent="0.25">
       <c r="L266">
         <v>49.184934771939872</v>
       </c>
@@ -17376,7 +17972,7 @@
         <v>0.39316239316239315</v>
       </c>
     </row>
-    <row r="267" spans="12:31">
+    <row r="267" spans="12:31" x14ac:dyDescent="0.25">
       <c r="M267">
         <v>7.8869227478220534</v>
       </c>
@@ -17426,7 +18022,7 @@
         <v>0.91025641025641024</v>
       </c>
     </row>
-    <row r="268" spans="12:31">
+    <row r="268" spans="12:31" x14ac:dyDescent="0.25">
       <c r="M268">
         <v>18.235534493730093</v>
       </c>
@@ -17476,7 +18072,7 @@
         <v>0.73575498575498566</v>
       </c>
     </row>
-    <row r="269" spans="12:31">
+    <row r="269" spans="12:31" x14ac:dyDescent="0.25">
       <c r="M269">
         <v>18.280814696448676</v>
       </c>
@@ -17526,7 +18122,7 @@
         <v>0.10683760683760685</v>
       </c>
     </row>
-    <row r="270" spans="12:31">
+    <row r="270" spans="12:31" x14ac:dyDescent="0.25">
       <c r="M270">
         <v>65.73070362641576</v>
       </c>
@@ -17576,7 +18172,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="271" spans="12:31">
+    <row r="271" spans="12:31" x14ac:dyDescent="0.25">
       <c r="M271">
         <v>37.621802032033088</v>
       </c>
@@ -17626,7 +18222,7 @@
         <v>1.7094017094017096E-2</v>
       </c>
     </row>
-    <row r="272" spans="12:31">
+    <row r="272" spans="12:31" x14ac:dyDescent="0.25">
       <c r="M272">
         <v>30.205516081811826</v>
       </c>
@@ -17676,7 +18272,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="273" spans="13:30">
+    <row r="273" spans="13:30" x14ac:dyDescent="0.25">
       <c r="M273">
         <v>38.775019254366008</v>
       </c>
@@ -17723,7 +18319,7 @@
         <v>0.10327635327635327</v>
       </c>
     </row>
-    <row r="274" spans="13:30">
+    <row r="274" spans="13:30" x14ac:dyDescent="0.25">
       <c r="M274">
         <v>35.033733710333095</v>
       </c>
@@ -17770,7 +18366,7 @@
         <v>0.15669515669515671</v>
       </c>
     </row>
-    <row r="275" spans="13:30">
+    <row r="275" spans="13:30" x14ac:dyDescent="0.25">
       <c r="M275">
         <v>48.869959300858795</v>
       </c>
@@ -17817,7 +18413,7 @@
         <v>0.38603988603988604</v>
       </c>
     </row>
-    <row r="276" spans="13:30">
+    <row r="276" spans="13:30" x14ac:dyDescent="0.25">
       <c r="M276">
         <v>32.859869541356368</v>
       </c>
@@ -17864,7 +18460,7 @@
         <v>0.50427350427350426</v>
       </c>
     </row>
-    <row r="277" spans="13:30">
+    <row r="277" spans="13:30" x14ac:dyDescent="0.25">
       <c r="N277">
         <v>5.912951108573858</v>
       </c>
@@ -17902,7 +18498,7 @@
         <v>0.16595441595441596</v>
       </c>
     </row>
-    <row r="278" spans="13:30">
+    <row r="278" spans="13:30" x14ac:dyDescent="0.25">
       <c r="N278">
         <v>21.451915263271427</v>
       </c>
@@ -17940,7 +18536,7 @@
         <v>2.0655270655270654E-2</v>
       </c>
     </row>
-    <row r="279" spans="13:30">
+    <row r="279" spans="13:30" x14ac:dyDescent="0.25">
       <c r="N279">
         <v>15.422679136353988</v>
       </c>
@@ -17978,7 +18574,7 @@
         <v>0.83618233618233617</v>
       </c>
     </row>
-    <row r="280" spans="13:30">
+    <row r="280" spans="13:30" x14ac:dyDescent="0.25">
       <c r="N280">
         <v>32.236375808046716</v>
       </c>
@@ -18016,7 +18612,7 @@
         <v>0.55698005698005693</v>
       </c>
     </row>
-    <row r="281" spans="13:30">
+    <row r="281" spans="13:30" x14ac:dyDescent="0.25">
       <c r="N281">
         <v>23.841676096963138</v>
       </c>
@@ -18054,7 +18650,7 @@
         <v>0.45441595441595439</v>
       </c>
     </row>
-    <row r="282" spans="13:30">
+    <row r="282" spans="13:30" x14ac:dyDescent="0.25">
       <c r="N282">
         <v>23.95101371982819</v>
       </c>
@@ -18092,7 +18688,7 @@
         <v>0.44871794871794873</v>
       </c>
     </row>
-    <row r="283" spans="13:30">
+    <row r="283" spans="13:30" x14ac:dyDescent="0.25">
       <c r="N283">
         <v>19.179641344244867</v>
       </c>
@@ -18130,7 +18726,7 @@
         <v>0.86894586894586889</v>
       </c>
     </row>
-    <row r="284" spans="13:30">
+    <row r="284" spans="13:30" x14ac:dyDescent="0.25">
       <c r="N284">
         <v>6.8639729909728269</v>
       </c>
@@ -18168,7 +18764,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="285" spans="13:30">
+    <row r="285" spans="13:30" x14ac:dyDescent="0.25">
       <c r="N285">
         <v>7.1136806012034679</v>
       </c>
@@ -18206,7 +18802,7 @@
         <v>0.63888888888888884</v>
       </c>
     </row>
-    <row r="286" spans="13:30">
+    <row r="286" spans="13:30" x14ac:dyDescent="0.25">
       <c r="N286">
         <v>7.2464604537690951</v>
       </c>
@@ -18244,7 +18840,7 @@
         <v>0.45584045584045585</v>
       </c>
     </row>
-    <row r="287" spans="13:30">
+    <row r="287" spans="13:30" x14ac:dyDescent="0.25">
       <c r="N287">
         <v>20.29540046465609</v>
       </c>
@@ -18282,7 +18878,7 @@
         <v>0.16595441595441596</v>
       </c>
     </row>
-    <row r="288" spans="13:30">
+    <row r="288" spans="13:30" x14ac:dyDescent="0.25">
       <c r="N288">
         <v>25.198296520641868</v>
       </c>
@@ -18320,7 +18916,7 @@
         <v>7.1225071225071226E-3</v>
       </c>
     </row>
-    <row r="289" spans="14:30">
+    <row r="289" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N289">
         <v>22.512412796474464</v>
       </c>
@@ -18358,7 +18954,7 @@
         <v>0.61538461538461542</v>
       </c>
     </row>
-    <row r="290" spans="14:30">
+    <row r="290" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N290">
         <v>15.08102999431415</v>
       </c>
@@ -18396,7 +18992,7 @@
         <v>4.3447293447293443E-2</v>
       </c>
     </row>
-    <row r="291" spans="14:30">
+    <row r="291" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N291">
         <v>29.275144372146698</v>
       </c>
@@ -18434,7 +19030,7 @@
         <v>0.34829059829059827</v>
       </c>
     </row>
-    <row r="292" spans="14:30">
+    <row r="292" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N292">
         <v>27.626035647751216</v>
       </c>
@@ -18472,7 +19068,7 @@
         <v>0.65028490028490027</v>
       </c>
     </row>
-    <row r="293" spans="14:30">
+    <row r="293" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N293">
         <v>30.276836120970781</v>
       </c>
@@ -18510,7 +19106,7 @@
         <v>0.86538461538461542</v>
       </c>
     </row>
-    <row r="294" spans="14:30">
+    <row r="294" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N294">
         <v>25.503049578710218</v>
       </c>
@@ -18548,7 +19144,7 @@
         <v>0.9814814814814814</v>
       </c>
     </row>
-    <row r="295" spans="14:30">
+    <row r="295" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N295">
         <v>27.438277007606775</v>
       </c>
@@ -18586,7 +19182,7 @@
         <v>0.17592592592592593</v>
       </c>
     </row>
-    <row r="296" spans="14:30">
+    <row r="296" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N296">
         <v>4.2426139787347594</v>
       </c>
@@ -18624,7 +19220,7 @@
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
-    <row r="297" spans="14:30">
+    <row r="297" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N297">
         <v>28.845715137713363</v>
       </c>
@@ -18662,7 +19258,7 @@
         <v>0.22934472934472935</v>
       </c>
     </row>
-    <row r="298" spans="14:30">
+    <row r="298" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N298">
         <v>25.57071487342688</v>
       </c>
@@ -18691,7 +19287,7 @@
         <v>8.5470085470085479E-3</v>
       </c>
     </row>
-    <row r="299" spans="14:30">
+    <row r="299" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N299">
         <v>30.200787352942875</v>
       </c>
@@ -18720,7 +19316,7 @@
         <v>0.88888888888888884</v>
       </c>
     </row>
-    <row r="300" spans="14:30">
+    <row r="300" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N300">
         <v>26.957076489844791</v>
       </c>
@@ -18749,7 +19345,7 @@
         <v>0.78418803418803418</v>
       </c>
     </row>
-    <row r="301" spans="14:30">
+    <row r="301" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N301">
         <v>29.486000551925127</v>
       </c>
@@ -18778,7 +19374,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="302" spans="14:30">
+    <row r="302" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N302">
         <v>6.0903179478529781</v>
       </c>
@@ -18807,7 +19403,7 @@
         <v>1.3532763532763533E-2</v>
       </c>
     </row>
-    <row r="303" spans="14:30">
+    <row r="303" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N303">
         <v>13.779362291181597</v>
       </c>
@@ -18836,7 +19432,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="304" spans="14:30">
+    <row r="304" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N304">
         <v>3.8306315419206758</v>
       </c>
@@ -18865,7 +19461,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="305" spans="14:30">
+    <row r="305" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N305">
         <v>28.236781437189439</v>
       </c>
@@ -18894,7 +19490,7 @@
         <v>0.6431623931623931</v>
       </c>
     </row>
-    <row r="306" spans="14:30">
+    <row r="306" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N306">
         <v>23.373477099125346</v>
       </c>
@@ -18923,7 +19519,7 @@
         <v>0.79985754985754987</v>
       </c>
     </row>
-    <row r="307" spans="14:30">
+    <row r="307" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N307">
         <v>4.8347207681619997</v>
       </c>
@@ -18952,7 +19548,7 @@
         <v>0.5242165242165242</v>
       </c>
     </row>
-    <row r="308" spans="14:30">
+    <row r="308" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N308">
         <v>22.989430546418333</v>
       </c>
@@ -18981,7 +19577,7 @@
         <v>5.6980056980056983E-3</v>
       </c>
     </row>
-    <row r="309" spans="14:30">
+    <row r="309" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N309">
         <v>13.943444486280676</v>
       </c>
@@ -19010,7 +19606,7 @@
         <v>0.12962962962962962</v>
       </c>
     </row>
-    <row r="310" spans="14:30">
+    <row r="310" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N310">
         <v>35.870255950645564</v>
       </c>
@@ -19039,7 +19635,7 @@
         <v>0.68091168091168086</v>
       </c>
     </row>
-    <row r="311" spans="14:30">
+    <row r="311" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N311">
         <v>32.79218960595199</v>
       </c>
@@ -19068,7 +19664,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="312" spans="14:30">
+    <row r="312" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N312">
         <v>33.74031416220577</v>
       </c>
@@ -19097,7 +19693,7 @@
         <v>0.51994301994301995</v>
       </c>
     </row>
-    <row r="313" spans="14:30">
+    <row r="313" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N313">
         <v>21.400060081009329</v>
       </c>
@@ -19126,7 +19722,7 @@
         <v>0.93376068376068377</v>
       </c>
     </row>
-    <row r="314" spans="14:30">
+    <row r="314" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N314">
         <v>4.3202629129059584</v>
       </c>
@@ -19155,7 +19751,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="315" spans="14:30">
+    <row r="315" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N315">
         <v>23.58702546859837</v>
       </c>
@@ -19181,7 +19777,7 @@
         <v>0.96438746438746437</v>
       </c>
     </row>
-    <row r="316" spans="14:30">
+    <row r="316" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N316">
         <v>22.393675182879896</v>
       </c>
@@ -19207,7 +19803,7 @@
         <v>0.579059829059829</v>
       </c>
     </row>
-    <row r="317" spans="14:30">
+    <row r="317" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N317">
         <v>38.813243789859683</v>
       </c>
@@ -19233,7 +19829,7 @@
         <v>0.97008547008547008</v>
       </c>
     </row>
-    <row r="318" spans="14:30">
+    <row r="318" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N318">
         <v>5.1891874637380466</v>
       </c>
@@ -19259,7 +19855,7 @@
         <v>0.48717948717948723</v>
       </c>
     </row>
-    <row r="319" spans="14:30">
+    <row r="319" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N319">
         <v>42.110574931976366</v>
       </c>
@@ -19285,7 +19881,7 @@
         <v>0.52279202279202286</v>
       </c>
     </row>
-    <row r="320" spans="14:30">
+    <row r="320" spans="14:30" x14ac:dyDescent="0.25">
       <c r="N320">
         <v>20.924467613961173</v>
       </c>
@@ -19311,7 +19907,7 @@
         <v>8.9743589743589744E-2</v>
       </c>
     </row>
-    <row r="321" spans="14:29">
+    <row r="321" spans="14:29" x14ac:dyDescent="0.25">
       <c r="N321">
         <v>29.474718968239312</v>
       </c>
@@ -19334,7 +19930,7 @@
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="322" spans="14:29">
+    <row r="322" spans="14:29" x14ac:dyDescent="0.25">
       <c r="N322">
         <v>26.224348798645149</v>
       </c>
@@ -19357,202 +19953,202 @@
         <v>7.7635327635327628E-2</v>
       </c>
     </row>
-    <row r="323" spans="14:29">
+    <row r="323" spans="14:29" x14ac:dyDescent="0.25">
       <c r="AC323">
         <v>0.8383190883190883</v>
       </c>
     </row>
-    <row r="324" spans="14:29">
+    <row r="324" spans="14:29" x14ac:dyDescent="0.25">
       <c r="AC324">
         <v>0.25213675213675213</v>
       </c>
     </row>
-    <row r="325" spans="14:29">
+    <row r="325" spans="14:29" x14ac:dyDescent="0.25">
       <c r="AC325">
         <v>0.69586894586894577</v>
       </c>
     </row>
-    <row r="326" spans="14:29">
+    <row r="326" spans="14:29" x14ac:dyDescent="0.25">
       <c r="AC326">
         <v>0.13176638176638178</v>
       </c>
     </row>
-    <row r="327" spans="14:29">
+    <row r="327" spans="14:29" x14ac:dyDescent="0.25">
       <c r="AC327">
         <v>0.41239316239316237</v>
       </c>
     </row>
-    <row r="328" spans="14:29">
+    <row r="328" spans="14:29" x14ac:dyDescent="0.25">
       <c r="AC328">
         <v>0.63532763532763536</v>
       </c>
     </row>
-    <row r="329" spans="14:29">
+    <row r="329" spans="14:29" x14ac:dyDescent="0.25">
       <c r="AC329">
         <v>0.40527065527065526</v>
       </c>
     </row>
-    <row r="330" spans="14:29">
+    <row r="330" spans="14:29" x14ac:dyDescent="0.25">
       <c r="AC330">
         <v>0.24287749287749288</v>
       </c>
     </row>
-    <row r="331" spans="14:29">
+    <row r="331" spans="14:29" x14ac:dyDescent="0.25">
       <c r="AC331">
         <v>0.65669515669515666</v>
       </c>
     </row>
-    <row r="332" spans="14:29">
+    <row r="332" spans="14:29" x14ac:dyDescent="0.25">
       <c r="AC332">
         <v>0.57692307692307687</v>
       </c>
     </row>
-    <row r="333" spans="14:29">
+    <row r="333" spans="14:29" x14ac:dyDescent="0.25">
       <c r="AC333">
         <v>0.57478632478632474</v>
       </c>
     </row>
-    <row r="334" spans="14:29">
+    <row r="334" spans="14:29" x14ac:dyDescent="0.25">
       <c r="AC334">
         <v>7.5498575498575499E-2</v>
       </c>
     </row>
-    <row r="335" spans="14:29">
+    <row r="335" spans="14:29" x14ac:dyDescent="0.25">
       <c r="AC335">
         <v>0.32549857549857553</v>
       </c>
     </row>
-    <row r="336" spans="14:29">
+    <row r="336" spans="14:29" x14ac:dyDescent="0.25">
       <c r="AC336">
         <v>0.13390313390313391</v>
       </c>
     </row>
-    <row r="337" spans="29:29">
+    <row r="337" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC337">
         <v>0.52492877492877499</v>
       </c>
     </row>
-    <row r="338" spans="29:29">
+    <row r="338" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC338">
         <v>6.4102564102564109E-3</v>
       </c>
     </row>
-    <row r="339" spans="29:29">
+    <row r="339" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC339">
         <v>1.1396011396011397E-2</v>
       </c>
     </row>
-    <row r="340" spans="29:29">
+    <row r="340" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC340">
         <v>0.74643874643874641</v>
       </c>
     </row>
-    <row r="341" spans="29:29">
+    <row r="341" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC341">
         <v>2.2079772079772082E-2</v>
       </c>
     </row>
-    <row r="342" spans="29:29">
+    <row r="342" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC342">
         <v>0.4131054131054131</v>
       </c>
     </row>
-    <row r="343" spans="29:29">
+    <row r="343" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC343">
         <v>0.24287749287749288</v>
       </c>
     </row>
-    <row r="344" spans="29:29">
+    <row r="344" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC344">
         <v>0.33119658119658119</v>
       </c>
     </row>
-    <row r="345" spans="29:29">
+    <row r="345" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC345">
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="346" spans="29:29">
+    <row r="346" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC346">
         <v>0.19230769230769229</v>
       </c>
     </row>
-    <row r="347" spans="29:29">
+    <row r="347" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC347">
         <v>0.36324786324786329</v>
       </c>
     </row>
-    <row r="348" spans="29:29">
+    <row r="348" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC348">
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="349" spans="29:29">
+    <row r="349" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC349">
         <v>0.81908831908831914</v>
       </c>
     </row>
-    <row r="350" spans="29:29">
+    <row r="350" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC350">
         <v>0.26851851851851849</v>
       </c>
     </row>
-    <row r="351" spans="29:29">
+    <row r="351" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC351">
         <v>0.68447293447293456</v>
       </c>
     </row>
-    <row r="352" spans="29:29">
+    <row r="352" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC352">
         <v>0.42307692307692313</v>
       </c>
     </row>
-    <row r="353" spans="29:29">
+    <row r="353" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC353">
         <v>0.79914529914529919</v>
       </c>
     </row>
-    <row r="354" spans="29:29">
+    <row r="354" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC354">
         <v>0.96438746438746437</v>
       </c>
     </row>
-    <row r="355" spans="29:29">
+    <row r="355" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC355">
         <v>0.25</v>
       </c>
     </row>
-    <row r="356" spans="29:29">
+    <row r="356" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC356">
         <v>0.65527065527065531</v>
       </c>
     </row>
-    <row r="357" spans="29:29">
+    <row r="357" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC357">
         <v>0.58974358974358976</v>
       </c>
     </row>
-    <row r="358" spans="29:29">
+    <row r="358" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC358">
         <v>2.6353276353276354E-2</v>
       </c>
     </row>
-    <row r="359" spans="29:29">
+    <row r="359" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC359">
         <v>0.41239316239316237</v>
       </c>
     </row>
-    <row r="360" spans="29:29">
+    <row r="360" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC360">
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="361" spans="29:29">
+    <row r="361" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC361">
         <v>1.4245014245014246E-3</v>
       </c>
     </row>
-    <row r="362" spans="29:29">
+    <row r="362" spans="29:29" x14ac:dyDescent="0.25">
       <c r="AC362">
         <v>1.4245014245014246E-3</v>
       </c>

</xml_diff>